<commit_message>
playing around with strength analysis
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,15 +476,20 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>0.1% Design Strength</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>elastic_mod_mean</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_std</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_CV</t>
         </is>
@@ -518,12 +523,15 @@
         <v>3.732721538111613</v>
       </c>
       <c r="I2" t="n">
+        <v>23.20243803640314</v>
+      </c>
+      <c r="J2" t="n">
         <v>40.27403487099166</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>3.364066935243426</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>8.352942400778611</v>
       </c>
     </row>
@@ -555,12 +563,15 @@
         <v>3.462820561380488</v>
       </c>
       <c r="I3" t="n">
+        <v>33.07472848284672</v>
+      </c>
+      <c r="J3" t="n">
         <v>88.02649052883081</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>17.67396567275773</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>20.07800784352419</v>
       </c>
     </row>
@@ -592,12 +603,15 @@
         <v>7.827709892680903</v>
       </c>
       <c r="I4" t="n">
+        <v>55.52712910140356</v>
+      </c>
+      <c r="J4" t="n">
         <v>45.05307813845685</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>2.882351201865095</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>6.397678740189672</v>
       </c>
     </row>
@@ -629,12 +643,15 @@
         <v>8.678824106185585</v>
       </c>
       <c r="I5" t="n">
+        <v>36.58608608616619</v>
+      </c>
+      <c r="J5" t="n">
         <v>17.21490344390057</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>2.463546693298648</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>14.31054609935387</v>
       </c>
     </row>
@@ -666,12 +683,15 @@
         <v>4.431981796208421</v>
       </c>
       <c r="I6" t="n">
+        <v>13.69604116136211</v>
+      </c>
+      <c r="J6" t="n">
         <v>11.14700398108137</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>2.88827239252185</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>25.91075052474916</v>
       </c>
     </row>
@@ -692,11 +712,12 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
         <v>11.61284885745432</v>
       </c>
-      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -715,11 +736,12 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
         <v>7.008953230507884</v>
       </c>
-      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -738,11 +760,12 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
         <v>8.56661207435533</v>
       </c>
-      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -761,11 +784,12 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
         <v>3.455792492327037</v>
       </c>
-      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -784,11 +808,12 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
         <v>11.86373934705964</v>
       </c>
-      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -818,50 +843,16 @@
         <v>7.993089968854619</v>
       </c>
       <c r="I12" t="n">
+        <v>37.36461920746228</v>
+      </c>
+      <c r="J12" t="n">
         <v>25.85486850181282</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>2.047709520089304</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>7.920015218587278</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1.589024858207071</v>
-      </c>
-      <c r="D13" t="n">
-        <v>104.9206363725</v>
-      </c>
-      <c r="E13" t="n">
-        <v>28.96061491177846</v>
-      </c>
-      <c r="F13" t="n">
-        <v>27.60240112246318</v>
-      </c>
-      <c r="G13" t="n">
-        <v>116.8148091253618</v>
-      </c>
-      <c r="H13" t="n">
-        <v>3.458469265995255</v>
-      </c>
-      <c r="I13" t="n">
-        <v>21.75123484725557</v>
-      </c>
-      <c r="J13" t="n">
-        <v>4.315906884542698</v>
-      </c>
-      <c r="K13" t="n">
-        <v>19.84212351551733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to do strength scaling with size, didnt work
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,30 +466,70 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>support_span</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Beta</t>
+          <t>load_span</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>char_strength</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>weibull_modulus</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>0.1% Design Strength</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>mean_gage_V</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>mean_gage_SA</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>mean_effective_V</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>mean_effective_SA</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>SA_series_scale_param</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>V_series_scale_param</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_mean</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_std</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_CV</t>
         </is>
@@ -517,21 +557,45 @@
         <v>27.81452307344672</v>
       </c>
       <c r="G2" t="n">
+        <v>185</v>
+      </c>
+      <c r="H2" t="n">
+        <v>70</v>
+      </c>
+      <c r="I2" t="n">
         <v>147.6313386352384</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>3.732721538111613</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>23.20243803640314</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
+        <v>4001.743631878642</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3050.109475517258</v>
+      </c>
+      <c r="N2" t="n">
+        <v>137.5265212300033</v>
+      </c>
+      <c r="O2" t="n">
+        <v>300.4577935658554</v>
+      </c>
+      <c r="P2" t="n">
+        <v>44356.98626751734</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>20303.22442703292</v>
+      </c>
+      <c r="R2" t="n">
         <v>40.27403487099166</v>
       </c>
-      <c r="K2" t="n">
+      <c r="S2" t="n">
         <v>3.364066935243426</v>
       </c>
-      <c r="L2" t="n">
+      <c r="T2" t="n">
         <v>8.352942400778611</v>
       </c>
     </row>
@@ -557,21 +621,45 @@
         <v>29.10135792551929</v>
       </c>
       <c r="G3" t="n">
+        <v>146</v>
+      </c>
+      <c r="H3" t="n">
+        <v>90</v>
+      </c>
+      <c r="I3" t="n">
         <v>243.0968542786452</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>3.462820561380488</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>33.07472848284672</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
+        <v>303.7279309294768</v>
+      </c>
+      <c r="M3" t="n">
+        <v>746.4895383827387</v>
+      </c>
+      <c r="N3" t="n">
+        <v>15.59242455167278</v>
+      </c>
+      <c r="O3" t="n">
+        <v>104.6741842613235</v>
+      </c>
+      <c r="P3" t="n">
+        <v>25445.96491811102</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3790.469359088768</v>
+      </c>
+      <c r="R3" t="n">
         <v>88.02649052883081</v>
       </c>
-      <c r="K3" t="n">
+      <c r="S3" t="n">
         <v>17.67396567275773</v>
       </c>
-      <c r="L3" t="n">
+      <c r="T3" t="n">
         <v>20.07800784352419</v>
       </c>
     </row>
@@ -597,21 +685,45 @@
         <v>14.23943744341875</v>
       </c>
       <c r="G4" t="n">
+        <v>185</v>
+      </c>
+      <c r="H4" t="n">
+        <v>70</v>
+      </c>
+      <c r="I4" t="n">
         <v>134.1934515757539</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>7.827709892680903</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>55.52712910140356</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
+        <v>2280.817582212344</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2302.69316730171</v>
+      </c>
+      <c r="N4" t="n">
+        <v>28.77239337819473</v>
+      </c>
+      <c r="O4" t="n">
+        <v>142.7393917410353</v>
+      </c>
+      <c r="P4" t="n">
+        <v>19154.69165355318</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>3861.066777515316</v>
+      </c>
+      <c r="R4" t="n">
         <v>45.05307813845685</v>
       </c>
-      <c r="K4" t="n">
+      <c r="S4" t="n">
         <v>2.882351201865095</v>
       </c>
-      <c r="L4" t="n">
+      <c r="T4" t="n">
         <v>6.397678740189672</v>
       </c>
     </row>
@@ -637,21 +749,45 @@
         <v>11.75472054835938</v>
       </c>
       <c r="G5" t="n">
+        <v>185</v>
+      </c>
+      <c r="H5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I5" t="n">
         <v>81.08861249799605</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>8.678824106185585</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>36.58608608616619</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
+        <v>37803.35499241169</v>
+      </c>
+      <c r="M5" t="n">
+        <v>9374.669557944622</v>
+      </c>
+      <c r="N5" t="n">
+        <v>276.8699166878031</v>
+      </c>
+      <c r="O5" t="n">
+        <v>366.6020013147311</v>
+      </c>
+      <c r="P5" t="n">
+        <v>29727.24762560007</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>22450.99738664972</v>
+      </c>
+      <c r="R5" t="n">
         <v>17.21490344390057</v>
       </c>
-      <c r="K5" t="n">
+      <c r="S5" t="n">
         <v>2.463546693298648</v>
       </c>
-      <c r="L5" t="n">
+      <c r="T5" t="n">
         <v>14.31054609935387</v>
       </c>
     </row>
@@ -677,21 +813,45 @@
         <v>21.49376010501468</v>
       </c>
       <c r="G6" t="n">
+        <v>185</v>
+      </c>
+      <c r="H6" t="n">
+        <v>40</v>
+      </c>
+      <c r="I6" t="n">
         <v>65.07948742504992</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>4.431981796208421</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>13.69604116136211</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
+        <v>85268.60956677426</v>
+      </c>
+      <c r="M6" t="n">
+        <v>14079.44017614436</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1712.765360158157</v>
+      </c>
+      <c r="O6" t="n">
+        <v>909.5129508948302</v>
+      </c>
+      <c r="P6" t="n">
+        <v>59190.63665068014</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>111465.8917184739</v>
+      </c>
+      <c r="R6" t="n">
         <v>11.14700398108137</v>
       </c>
-      <c r="K6" t="n">
+      <c r="S6" t="n">
         <v>2.88827239252185</v>
       </c>
-      <c r="L6" t="n">
+      <c r="T6" t="n">
         <v>25.91075052474916</v>
       </c>
     </row>
@@ -710,14 +870,30 @@
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>146</v>
+      </c>
+      <c r="H7" t="n">
+        <v>24</v>
+      </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>46050.90522239159</v>
+      </c>
+      <c r="M7" t="n">
+        <v>9191.79744957916</v>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
         <v>11.61284885745432</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -734,14 +910,30 @@
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>146</v>
+      </c>
+      <c r="H8" t="n">
+        <v>24</v>
+      </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>65773.92710294698</v>
+      </c>
+      <c r="M8" t="n">
+        <v>10985.20703180743</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="n">
         <v>7.008953230507884</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -758,14 +950,30 @@
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>146</v>
+      </c>
+      <c r="H9" t="n">
+        <v>24</v>
+      </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>127766.0304164031</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15310.48896541679</v>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
         <v>8.56661207435533</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -782,14 +990,30 @@
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>146</v>
+      </c>
+      <c r="H10" t="n">
+        <v>24</v>
+      </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>83593.06812304401</v>
+      </c>
+      <c r="M10" t="n">
+        <v>12384.15824045096</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="n">
         <v>3.455792492327037</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -806,14 +1030,30 @@
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>146</v>
+      </c>
+      <c r="H11" t="n">
+        <v>24</v>
+      </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>99451.95742906225</v>
+      </c>
+      <c r="M11" t="n">
+        <v>13507.90593264003</v>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="n">
         <v>11.86373934705964</v>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -837,21 +1077,45 @@
         <v>14.70815602602536</v>
       </c>
       <c r="G12" t="n">
+        <v>130</v>
+      </c>
+      <c r="H12" t="n">
+        <v>70</v>
+      </c>
+      <c r="I12" t="n">
         <v>88.66609260977411</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>7.993089968854619</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>37.36461920746228</v>
       </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
+        <v>1275.209927873813</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1443.336022352533</v>
+      </c>
+      <c r="N12" t="n">
+        <v>20.58771781284712</v>
+      </c>
+      <c r="O12" t="n">
+        <v>116.4296988845964</v>
+      </c>
+      <c r="P12" t="n">
+        <v>10323.36646382974</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1825.432494217799</v>
+      </c>
+      <c r="R12" t="n">
         <v>25.85486850181282</v>
       </c>
-      <c r="K12" t="n">
+      <c r="S12" t="n">
         <v>2.047709520089304</v>
       </c>
-      <c r="L12" t="n">
+      <c r="T12" t="n">
         <v>7.920015218587278</v>
       </c>
     </row>

</xml_diff>

<commit_message>
back to scaling on probability with effective size
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,10 +584,10 @@
         <v>300.4577935658554</v>
       </c>
       <c r="P2" t="n">
-        <v>44356.98626751734</v>
+        <v>680.7369728571302</v>
       </c>
       <c r="Q2" t="n">
-        <v>20303.22442703292</v>
+        <v>552.1467546469989</v>
       </c>
       <c r="R2" t="n">
         <v>40.27403487099166</v>
@@ -648,10 +648,10 @@
         <v>104.6741842613235</v>
       </c>
       <c r="P3" t="n">
-        <v>25445.96491811102</v>
+        <v>931.2633461952848</v>
       </c>
       <c r="Q3" t="n">
-        <v>3790.469359088768</v>
+        <v>537.3673108146872</v>
       </c>
       <c r="R3" t="n">
         <v>88.02649052883081</v>
@@ -712,10 +712,10 @@
         <v>142.7393917410353</v>
       </c>
       <c r="P4" t="n">
-        <v>19154.69165355318</v>
+        <v>252.9164449060363</v>
       </c>
       <c r="Q4" t="n">
-        <v>3861.066777515316</v>
+        <v>206.1186936916146</v>
       </c>
       <c r="R4" t="n">
         <v>45.05307813845685</v>
@@ -776,10 +776,10 @@
         <v>366.6020013147311</v>
       </c>
       <c r="P5" t="n">
-        <v>29727.24762560007</v>
+        <v>160.1083736445783</v>
       </c>
       <c r="Q5" t="n">
-        <v>22450.99738664972</v>
+        <v>155.0123028439635</v>
       </c>
       <c r="R5" t="n">
         <v>17.21490344390057</v>
@@ -840,10 +840,10 @@
         <v>909.5129508948302</v>
       </c>
       <c r="P6" t="n">
-        <v>59190.63665068014</v>
+        <v>302.7249032640486</v>
       </c>
       <c r="Q6" t="n">
-        <v>111465.8917184739</v>
+        <v>349.1982764246479</v>
       </c>
       <c r="R6" t="n">
         <v>11.14700398108137</v>
@@ -1055,70 +1055,6 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>3.5340625</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.03035907421343368</v>
-      </c>
-      <c r="D12" t="n">
-        <v>83.59120132718751</v>
-      </c>
-      <c r="E12" t="n">
-        <v>12.29472431523172</v>
-      </c>
-      <c r="F12" t="n">
-        <v>14.70815602602536</v>
-      </c>
-      <c r="G12" t="n">
-        <v>130</v>
-      </c>
-      <c r="H12" t="n">
-        <v>70</v>
-      </c>
-      <c r="I12" t="n">
-        <v>88.66609260977411</v>
-      </c>
-      <c r="J12" t="n">
-        <v>7.993089968854619</v>
-      </c>
-      <c r="K12" t="n">
-        <v>37.36461920746228</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1275.209927873813</v>
-      </c>
-      <c r="M12" t="n">
-        <v>1443.336022352533</v>
-      </c>
-      <c r="N12" t="n">
-        <v>20.58771781284712</v>
-      </c>
-      <c r="O12" t="n">
-        <v>116.4296988845964</v>
-      </c>
-      <c r="P12" t="n">
-        <v>10323.36646382974</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>1825.432494217799</v>
-      </c>
-      <c r="R12" t="n">
-        <v>25.85486850181282</v>
-      </c>
-      <c r="S12" t="n">
-        <v>2.047709520089304</v>
-      </c>
-      <c r="T12" t="n">
-        <v>7.920015218587278</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add logarithm and cross section size to elastic calcs
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,16 @@
           <t>elastic_mod_CV</t>
         </is>
       </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>log_elastic_mod_mean</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>cross_section</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -598,6 +608,12 @@
       <c r="T2" t="n">
         <v>8.352942400778611</v>
       </c>
+      <c r="U2" t="n">
+        <v>1.605025141761029</v>
+      </c>
+      <c r="V2" t="n">
+        <v>21.63104665880347</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -662,6 +678,12 @@
       <c r="T3" t="n">
         <v>20.07800784352419</v>
       </c>
+      <c r="U3" t="n">
+        <v>1.944613387595852</v>
+      </c>
+      <c r="V3" t="n">
+        <v>2.080328294037512</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -726,6 +748,12 @@
       <c r="T4" t="n">
         <v>6.397678740189672</v>
       </c>
+      <c r="U4" t="n">
+        <v>1.653724468408931</v>
+      </c>
+      <c r="V4" t="n">
+        <v>12.32874368763429</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -790,6 +818,12 @@
       <c r="T5" t="n">
         <v>14.31054609935387</v>
       </c>
+      <c r="U5" t="n">
+        <v>1.235904591147647</v>
+      </c>
+      <c r="V5" t="n">
+        <v>204.3424594184416</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -853,6 +887,12 @@
       </c>
       <c r="T6" t="n">
         <v>25.91075052474916</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1.047158156233841</v>
+      </c>
+      <c r="V6" t="n">
+        <v>460.9114030636447</v>
       </c>
     </row>
     <row r="7">
@@ -894,6 +934,12 @@
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
+      <c r="U7" t="n">
+        <v>1.064938773683436</v>
+      </c>
+      <c r="V7" t="n">
+        <v>315.4171590574766</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -934,6 +980,12 @@
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
+      <c r="U8" t="n">
+        <v>0.8456531620237618</v>
+      </c>
+      <c r="V8" t="n">
+        <v>450.5063500201848</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -974,6 +1026,12 @@
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
+      <c r="U9" t="n">
+        <v>0.932809100998973</v>
+      </c>
+      <c r="V9" t="n">
+        <v>875.1097973726238</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1014,6 +1072,12 @@
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
+        <v>0.538547656797904</v>
+      </c>
+      <c r="V10" t="n">
+        <v>572.5552611167398</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1054,6 +1118,82 @@
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
+      <c r="U11" t="n">
+        <v>1.074221596434249</v>
+      </c>
+      <c r="V11" t="n">
+        <v>681.1777906100154</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3.5340625</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.03035907421343368</v>
+      </c>
+      <c r="D12" t="n">
+        <v>83.59120132718751</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12.29472431523172</v>
+      </c>
+      <c r="F12" t="n">
+        <v>14.70815602602536</v>
+      </c>
+      <c r="G12" t="n">
+        <v>130</v>
+      </c>
+      <c r="H12" t="n">
+        <v>70</v>
+      </c>
+      <c r="I12" t="n">
+        <v>88.66609260977411</v>
+      </c>
+      <c r="J12" t="n">
+        <v>7.993089968854619</v>
+      </c>
+      <c r="K12" t="n">
+        <v>37.36461920746228</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1275.209927873813</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1443.336022352533</v>
+      </c>
+      <c r="N12" t="n">
+        <v>20.58771781284712</v>
+      </c>
+      <c r="O12" t="n">
+        <v>116.4296988845964</v>
+      </c>
+      <c r="P12" t="n">
+        <v>160.7825106960555</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>129.4495508456753</v>
+      </c>
+      <c r="R12" t="n">
+        <v>25.85486850181282</v>
+      </c>
+      <c r="S12" t="n">
+        <v>2.047709520089304</v>
+      </c>
+      <c r="T12" t="n">
+        <v>7.920015218587278</v>
+      </c>
+      <c r="U12" t="n">
+        <v>1.412542333286495</v>
+      </c>
+      <c r="V12" t="n">
+        <v>9.809307137490865</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
some more analysis and editing plots
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>0.1% Design Strength</t>
+          <t>Design Strength</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -558,13 +558,13 @@
         <v>0.07254117604658906</v>
       </c>
       <c r="D2" t="n">
-        <v>138.8755041666772</v>
+        <v>133.465852319</v>
       </c>
       <c r="E2" t="n">
-        <v>31.03739216765115</v>
+        <v>37.12289028844057</v>
       </c>
       <c r="F2" t="n">
-        <v>22.34907614117486</v>
+        <v>27.81452307344672</v>
       </c>
       <c r="G2" t="n">
         <v>185</v>
@@ -573,13 +573,13 @@
         <v>70</v>
       </c>
       <c r="I2" t="n">
-        <v>150.3364152022824</v>
+        <v>147.6313386352384</v>
       </c>
       <c r="J2" t="n">
-        <v>5.121031397069969</v>
+        <v>3.732721538111613</v>
       </c>
       <c r="K2" t="n">
-        <v>39.01998707197287</v>
+        <v>43.04876000792099</v>
       </c>
       <c r="L2" t="n">
         <v>4001.743631878642</v>
@@ -588,16 +588,16 @@
         <v>3050.109475517258</v>
       </c>
       <c r="N2" t="n">
-        <v>90.58918618971465</v>
+        <v>137.5265212300033</v>
       </c>
       <c r="O2" t="n">
-        <v>245.841630751515</v>
+        <v>300.4577935658554</v>
       </c>
       <c r="P2" t="n">
-        <v>440.4484012220136</v>
+        <v>680.7369728571302</v>
       </c>
       <c r="Q2" t="n">
-        <v>362.4337907205943</v>
+        <v>552.1467546469989</v>
       </c>
       <c r="R2" t="n">
         <v>40.27403487099166</v>
@@ -628,13 +628,13 @@
         <v>0.1158508893855743</v>
       </c>
       <c r="D3" t="n">
-        <v>218.8138713827705</v>
+        <v>218.92485695</v>
       </c>
       <c r="E3" t="n">
-        <v>63.67780790729131</v>
+        <v>63.71010620895059</v>
       </c>
       <c r="F3" t="n">
-        <v>29.10135792803552</v>
+        <v>29.10135792551929</v>
       </c>
       <c r="G3" t="n">
         <v>146</v>
@@ -643,13 +643,13 @@
         <v>90</v>
       </c>
       <c r="I3" t="n">
-        <v>242.9736146025795</v>
+        <v>243.0968542786452</v>
       </c>
       <c r="J3" t="n">
-        <v>3.462820725541309</v>
+        <v>3.462820561380488</v>
       </c>
       <c r="K3" t="n">
-        <v>33.05796414045407</v>
+        <v>64.3939687516219</v>
       </c>
       <c r="L3" t="n">
         <v>303.7279309294768</v>
@@ -658,16 +658,16 @@
         <v>746.4895383827387</v>
       </c>
       <c r="N3" t="n">
-        <v>15.59242369476238</v>
+        <v>15.59242455167278</v>
       </c>
       <c r="O3" t="n">
-        <v>104.6741816542787</v>
+        <v>104.6741842613235</v>
       </c>
       <c r="P3" t="n">
-        <v>930.7911696715574</v>
+        <v>931.2633461952848</v>
       </c>
       <c r="Q3" t="n">
-        <v>537.0948599206899</v>
+        <v>537.3673108146872</v>
       </c>
       <c r="R3" t="n">
         <v>88.02649052883081</v>
@@ -698,13 +698,13 @@
         <v>0.05245103536738928</v>
       </c>
       <c r="D4" t="n">
-        <v>134.8860297451756</v>
+        <v>126.70803296</v>
       </c>
       <c r="E4" t="n">
-        <v>15.73524028677134</v>
+        <v>18.0425110891256</v>
       </c>
       <c r="F4" t="n">
-        <v>11.66558191126101</v>
+        <v>14.23943744341875</v>
       </c>
       <c r="G4" t="n">
         <v>185</v>
@@ -713,13 +713,13 @@
         <v>70</v>
       </c>
       <c r="I4" t="n">
-        <v>141.4381450446304</v>
+        <v>134.1934515757539</v>
       </c>
       <c r="J4" t="n">
-        <v>9.768252025177432</v>
+        <v>7.827709892680903</v>
       </c>
       <c r="K4" t="n">
-        <v>69.7383082732908</v>
+        <v>74.56024459595899</v>
       </c>
       <c r="L4" t="n">
         <v>2280.817582212344</v>
@@ -728,16 +728,16 @@
         <v>2302.69316730171</v>
       </c>
       <c r="N4" t="n">
-        <v>21.03323866157426</v>
+        <v>28.77239337819473</v>
       </c>
       <c r="O4" t="n">
-        <v>124.9492445608842</v>
+        <v>142.7393917410353</v>
       </c>
       <c r="P4" t="n">
-        <v>231.8538619776552</v>
+        <v>252.9164449060363</v>
       </c>
       <c r="Q4" t="n">
-        <v>193.1949234037351</v>
+        <v>206.1186936916146</v>
       </c>
       <c r="R4" t="n">
         <v>45.05307813845685</v>
@@ -768,13 +768,13 @@
         <v>0.05597618541248907</v>
       </c>
       <c r="D5" t="n">
-        <v>81.12990751958198</v>
+        <v>77.15356611749999</v>
       </c>
       <c r="E5" t="n">
-        <v>8.18438136934744</v>
+        <v>9.069186090205813</v>
       </c>
       <c r="F5" t="n">
-        <v>10.08799543789941</v>
+        <v>11.75472054835938</v>
       </c>
       <c r="G5" t="n">
         <v>185</v>
@@ -783,13 +783,13 @@
         <v>40</v>
       </c>
       <c r="I5" t="n">
-        <v>83.86363352201379</v>
+        <v>81.08861249799605</v>
       </c>
       <c r="J5" t="n">
-        <v>13.00323292828877</v>
+        <v>8.678824106185585</v>
       </c>
       <c r="K5" t="n">
-        <v>49.3035880021238</v>
+        <v>47.72711205448898</v>
       </c>
       <c r="L5" t="n">
         <v>37803.35499241169</v>
@@ -798,16 +798,16 @@
         <v>9374.669557944622</v>
       </c>
       <c r="N5" t="n">
-        <v>148.8630956415505</v>
+        <v>276.8699166878031</v>
       </c>
       <c r="O5" t="n">
-        <v>276.9284188885694</v>
+        <v>366.6020013147311</v>
       </c>
       <c r="P5" t="n">
-        <v>129.2413214155434</v>
+        <v>160.1083736445783</v>
       </c>
       <c r="Q5" t="n">
-        <v>123.21670345754</v>
+        <v>155.0123028439635</v>
       </c>
       <c r="R5" t="n">
         <v>17.21490344390057</v>
@@ -838,13 +838,13 @@
         <v>0.09574271077563332</v>
       </c>
       <c r="D6" t="n">
-        <v>66.7999749474383</v>
+        <v>59.56530107250001</v>
       </c>
       <c r="E6" t="n">
-        <v>16.11904721528004</v>
+        <v>12.80282291835289</v>
       </c>
       <c r="F6" t="n">
-        <v>24.13031925231012</v>
+        <v>21.49376010501468</v>
       </c>
       <c r="G6" t="n">
         <v>185</v>
@@ -853,13 +853,13 @@
         <v>40</v>
       </c>
       <c r="I6" t="n">
-        <v>73.6480971540503</v>
+        <v>65.07948742504992</v>
       </c>
       <c r="J6" t="n">
-        <v>3.924745594045886</v>
+        <v>4.431981796208421</v>
       </c>
       <c r="K6" t="n">
-        <v>12.67173629148398</v>
+        <v>23.04998999891203</v>
       </c>
       <c r="L6" t="n">
         <v>85268.60956677426</v>
@@ -868,16 +868,16 @@
         <v>14079.44017614436</v>
       </c>
       <c r="N6" t="n">
-        <v>2042.805664096682</v>
+        <v>1712.765360158157</v>
       </c>
       <c r="O6" t="n">
-        <v>999.2242607099112</v>
+        <v>909.5129508948302</v>
       </c>
       <c r="P6" t="n">
-        <v>428.0124601965922</v>
+        <v>302.7249032640486</v>
       </c>
       <c r="Q6" t="n">
-        <v>513.5540380962364</v>
+        <v>349.1982764246479</v>
       </c>
       <c r="R6" t="n">
         <v>11.14700398108137</v>
@@ -906,7 +906,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>69.44860162714492</v>
+        <v>69.21942002999999</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -952,7 +952,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>74.58645854342882</v>
+        <v>74.62428989</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -998,7 +998,7 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>68.39672464721359</v>
+        <v>66.09967249</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -1036,15 +1036,15 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27</v>
+        <v>29.45</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>29.42122562767789</v>
+        <v>89.27432161999999</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -1058,141 +1058,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
-        <v>83593.06812304401</v>
+        <v>99451.95742906225</v>
       </c>
       <c r="M10" t="n">
-        <v>12384.15824045096</v>
+        <v>13507.90593264003</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>3.455792492327037</v>
+        <v>11.86373934705964</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
-        <v>0.538547656797904</v>
+        <v>1.074221596434249</v>
       </c>
       <c r="V10" t="n">
-        <v>572.5552611167398</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>29.45</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
-        <v>92.37672388423256</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
-        <v>146</v>
-      </c>
-      <c r="H11" t="n">
-        <v>24</v>
-      </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="n">
-        <v>99451.95742906225</v>
-      </c>
-      <c r="M11" t="n">
-        <v>13507.90593264003</v>
-      </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="n">
-        <v>11.86373934705964</v>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="n">
-        <v>1.074221596434249</v>
-      </c>
-      <c r="V11" t="n">
         <v>681.1777906100154</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>3.5340625</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.03035907421343368</v>
-      </c>
-      <c r="D12" t="n">
-        <v>83.59120132952999</v>
-      </c>
-      <c r="E12" t="n">
-        <v>12.2947243175728</v>
-      </c>
-      <c r="F12" t="n">
-        <v>14.70815602841382</v>
-      </c>
-      <c r="G12" t="n">
-        <v>130</v>
-      </c>
-      <c r="H12" t="n">
-        <v>70</v>
-      </c>
-      <c r="I12" t="n">
-        <v>88.66609260977411</v>
-      </c>
-      <c r="J12" t="n">
-        <v>7.993089968854619</v>
-      </c>
-      <c r="K12" t="n">
-        <v>37.36461920746228</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1275.209927873813</v>
-      </c>
-      <c r="M12" t="n">
-        <v>1443.336022352533</v>
-      </c>
-      <c r="N12" t="n">
-        <v>20.58771781284712</v>
-      </c>
-      <c r="O12" t="n">
-        <v>116.4296988845964</v>
-      </c>
-      <c r="P12" t="n">
-        <v>160.7825106960555</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>129.4495508456753</v>
-      </c>
-      <c r="R12" t="n">
-        <v>25.85486850181282</v>
-      </c>
-      <c r="S12" t="n">
-        <v>2.047709520089304</v>
-      </c>
-      <c r="T12" t="n">
-        <v>7.920015218587278</v>
-      </c>
-      <c r="U12" t="n">
-        <v>1.412542333286495</v>
-      </c>
-      <c r="V12" t="n">
-        <v>9.809307137490865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Size scaling in same plot
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,35 +511,25 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>SA_series_scale_param</t>
+          <t>elastic_mod_mean</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>V_series_scale_param</t>
+          <t>elastic_mod_std</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>elastic_mod_mean</t>
+          <t>elastic_mod_CV</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>elastic_mod_std</t>
+          <t>log_elastic_mod_mean</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>elastic_mod_CV</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>log_elastic_mod_mean</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>cross_section</t>
         </is>
@@ -594,24 +584,18 @@
         <v>104.6741842613235</v>
       </c>
       <c r="P2" t="n">
-        <v>931.2633461952848</v>
+        <v>88.02649052883081</v>
       </c>
       <c r="Q2" t="n">
-        <v>537.3673108146872</v>
+        <v>17.67396567275773</v>
       </c>
       <c r="R2" t="n">
-        <v>88.02649052883081</v>
+        <v>20.07800784352419</v>
       </c>
       <c r="S2" t="n">
-        <v>17.67396567275773</v>
+        <v>1.944613387595852</v>
       </c>
       <c r="T2" t="n">
-        <v>20.07800784352419</v>
-      </c>
-      <c r="U2" t="n">
-        <v>1.944613387595852</v>
-      </c>
-      <c r="V2" t="n">
         <v>2.080328294037512</v>
       </c>
     </row>
@@ -664,24 +648,18 @@
         <v>142.7393917410353</v>
       </c>
       <c r="P3" t="n">
-        <v>252.9164449060363</v>
+        <v>45.05307813845685</v>
       </c>
       <c r="Q3" t="n">
-        <v>206.1186936916146</v>
+        <v>2.882351201865095</v>
       </c>
       <c r="R3" t="n">
-        <v>45.05307813845685</v>
+        <v>6.397678740189672</v>
       </c>
       <c r="S3" t="n">
-        <v>2.882351201865095</v>
+        <v>1.653724468408931</v>
       </c>
       <c r="T3" t="n">
-        <v>6.397678740189672</v>
-      </c>
-      <c r="U3" t="n">
-        <v>1.653724468408931</v>
-      </c>
-      <c r="V3" t="n">
         <v>12.32874368763429</v>
       </c>
     </row>
@@ -734,24 +712,18 @@
         <v>300.4577935658554</v>
       </c>
       <c r="P4" t="n">
-        <v>680.7369728571302</v>
+        <v>40.27403487099166</v>
       </c>
       <c r="Q4" t="n">
-        <v>552.1467546469989</v>
+        <v>3.364066935243426</v>
       </c>
       <c r="R4" t="n">
-        <v>40.27403487099166</v>
+        <v>8.352942400778611</v>
       </c>
       <c r="S4" t="n">
-        <v>3.364066935243426</v>
+        <v>1.605025141761029</v>
       </c>
       <c r="T4" t="n">
-        <v>8.352942400778611</v>
-      </c>
-      <c r="U4" t="n">
-        <v>1.605025141761029</v>
-      </c>
-      <c r="V4" t="n">
         <v>21.63104665880347</v>
       </c>
     </row>
@@ -804,24 +776,18 @@
         <v>366.6020013147311</v>
       </c>
       <c r="P5" t="n">
-        <v>160.1083736445783</v>
+        <v>17.21490344390057</v>
       </c>
       <c r="Q5" t="n">
-        <v>155.0123028439635</v>
+        <v>2.463546693298648</v>
       </c>
       <c r="R5" t="n">
-        <v>17.21490344390057</v>
+        <v>14.31054609935387</v>
       </c>
       <c r="S5" t="n">
-        <v>2.463546693298648</v>
+        <v>1.235904591147647</v>
       </c>
       <c r="T5" t="n">
-        <v>14.31054609935387</v>
-      </c>
-      <c r="U5" t="n">
-        <v>1.235904591147647</v>
-      </c>
-      <c r="V5" t="n">
         <v>204.3424594184416</v>
       </c>
     </row>
@@ -857,17 +823,15 @@
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>11.61284885745432</v>
+      </c>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>11.61284885745432</v>
-      </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="n">
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="n">
         <v>1.064938773683436</v>
       </c>
-      <c r="V6" t="n">
+      <c r="T6" t="n">
         <v>315.4171590574766</v>
       </c>
     </row>
@@ -903,17 +867,15 @@
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>7.008953230507884</v>
+      </c>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
-        <v>7.008953230507884</v>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="n">
         <v>0.8456531620237618</v>
       </c>
-      <c r="V7" t="n">
+      <c r="T7" t="n">
         <v>450.5063500201848</v>
       </c>
     </row>
@@ -966,24 +928,18 @@
         <v>909.5129508948302</v>
       </c>
       <c r="P8" t="n">
-        <v>302.7249032640486</v>
+        <v>11.14700398108137</v>
       </c>
       <c r="Q8" t="n">
-        <v>349.1982764246479</v>
+        <v>2.88827239252185</v>
       </c>
       <c r="R8" t="n">
-        <v>11.14700398108137</v>
+        <v>25.91075052474916</v>
       </c>
       <c r="S8" t="n">
-        <v>2.88827239252185</v>
+        <v>1.047158156233841</v>
       </c>
       <c r="T8" t="n">
-        <v>25.91075052474916</v>
-      </c>
-      <c r="U8" t="n">
-        <v>1.047158156233841</v>
-      </c>
-      <c r="V8" t="n">
         <v>460.9114030636447</v>
       </c>
     </row>
@@ -1019,17 +975,15 @@
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>11.86373934705964</v>
+      </c>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="n">
-        <v>11.86373934705964</v>
-      </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="n">
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="n">
         <v>1.074221596434249</v>
       </c>
-      <c r="V9" t="n">
+      <c r="T9" t="n">
         <v>681.1777906100154</v>
       </c>
     </row>
@@ -1065,17 +1019,15 @@
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>8.56661207435533</v>
+      </c>
       <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="n">
-        <v>8.56661207435533</v>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="n">
         <v>0.932809100998973</v>
       </c>
-      <c r="V10" t="n">
+      <c r="T10" t="n">
         <v>875.1097973726238</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Confidence intervals and error bars
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,57 +481,87 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>char_strength_95%_upper</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>char_strength_95%_lower</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>weibull_modulus</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>weibull_modulus_95%_upper</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>weibull_modulus_95%_lower</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Design Strength</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>mean_gage_V</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>mean_gage_SA</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>mean_effective_V</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>mean_effective_SA</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_mean</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_std</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_CV</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>log_elastic_mod_mean</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>cross_section</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>char_strength_disp</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>weibull_modulus_disp</t>
         </is>
       </c>
     </row>
@@ -566,37 +596,61 @@
         <v>243.0968542786452</v>
       </c>
       <c r="J2" t="n">
+        <v>301.1757812192096</v>
+      </c>
+      <c r="K2" t="n">
+        <v>196.2179041121504</v>
+      </c>
+      <c r="L2" t="n">
         <v>3.462820561380488</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
+        <v>6.33233774559996</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.893633397658162</v>
+      </c>
+      <c r="O2" t="n">
         <v>64.3939687516219</v>
       </c>
-      <c r="L2" t="n">
+      <c r="P2" t="n">
         <v>303.7279309294768</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q2" t="n">
         <v>746.4895383827387</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>15.59242455167278</v>
       </c>
-      <c r="O2" t="n">
+      <c r="S2" t="n">
         <v>104.6741842613235</v>
       </c>
-      <c r="P2" t="n">
+      <c r="T2" t="n">
         <v>88.02649052883081</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="U2" t="n">
         <v>17.67396567275773</v>
       </c>
-      <c r="R2" t="n">
+      <c r="V2" t="n">
         <v>20.07800784352419</v>
       </c>
-      <c r="S2" t="n">
+      <c r="W2" t="n">
         <v>1.944613387595852</v>
       </c>
-      <c r="T2" t="n">
+      <c r="X2" t="n">
         <v>2.080328294037512</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>243
+(301,196)</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>3.5
+(6.3,1.9)</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -630,37 +684,61 @@
         <v>134.1934515757539</v>
       </c>
       <c r="J3" t="n">
+        <v>145.8141782341235</v>
+      </c>
+      <c r="K3" t="n">
+        <v>123.4988439663269</v>
+      </c>
+      <c r="L3" t="n">
         <v>7.827709892680903</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
+        <v>12.99038824738473</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4.716798374083251</v>
+      </c>
+      <c r="O3" t="n">
         <v>74.56024459595899</v>
       </c>
-      <c r="L3" t="n">
+      <c r="P3" t="n">
         <v>2280.817582212344</v>
       </c>
-      <c r="M3" t="n">
+      <c r="Q3" t="n">
         <v>2302.69316730171</v>
       </c>
-      <c r="N3" t="n">
+      <c r="R3" t="n">
         <v>28.77239337819473</v>
       </c>
-      <c r="O3" t="n">
+      <c r="S3" t="n">
         <v>142.7393917410353</v>
       </c>
-      <c r="P3" t="n">
+      <c r="T3" t="n">
         <v>45.05307813845685</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="U3" t="n">
         <v>2.882351201865095</v>
       </c>
-      <c r="R3" t="n">
+      <c r="V3" t="n">
         <v>6.397678740189672</v>
       </c>
-      <c r="S3" t="n">
+      <c r="W3" t="n">
         <v>1.653724468408931</v>
       </c>
-      <c r="T3" t="n">
+      <c r="X3" t="n">
         <v>12.32874368763429</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>134
+(146,123)</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>7.8
+(13.0,4.7)</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -694,37 +772,61 @@
         <v>147.6313386352384</v>
       </c>
       <c r="J4" t="n">
+        <v>176.0407780413132</v>
+      </c>
+      <c r="K4" t="n">
+        <v>123.8066111143724</v>
+      </c>
+      <c r="L4" t="n">
         <v>3.732721538111613</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
+        <v>6.257881243360847</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.226505991283302</v>
+      </c>
+      <c r="O4" t="n">
         <v>43.04876000792099</v>
       </c>
-      <c r="L4" t="n">
+      <c r="P4" t="n">
         <v>4001.743631878642</v>
       </c>
-      <c r="M4" t="n">
+      <c r="Q4" t="n">
         <v>3050.109475517258</v>
       </c>
-      <c r="N4" t="n">
+      <c r="R4" t="n">
         <v>137.5265212300033</v>
       </c>
-      <c r="O4" t="n">
+      <c r="S4" t="n">
         <v>300.4577935658554</v>
       </c>
-      <c r="P4" t="n">
+      <c r="T4" t="n">
         <v>40.27403487099166</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="U4" t="n">
         <v>3.364066935243426</v>
       </c>
-      <c r="R4" t="n">
+      <c r="V4" t="n">
         <v>8.352942400778611</v>
       </c>
-      <c r="S4" t="n">
+      <c r="W4" t="n">
         <v>1.605025141761029</v>
       </c>
-      <c r="T4" t="n">
+      <c r="X4" t="n">
         <v>21.63104665880347</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>148
+(176,124)</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>3.7
+(6.3,2.2)</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -758,37 +860,61 @@
         <v>81.08861249799605</v>
       </c>
       <c r="J5" t="n">
+        <v>91.56091174079913</v>
+      </c>
+      <c r="K5" t="n">
+        <v>71.81408476429806</v>
+      </c>
+      <c r="L5" t="n">
         <v>8.678824106185585</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
+        <v>19.78614227873543</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3.806805126791093</v>
+      </c>
+      <c r="O5" t="n">
         <v>47.72711205448898</v>
       </c>
-      <c r="L5" t="n">
+      <c r="P5" t="n">
         <v>37803.35499241169</v>
       </c>
-      <c r="M5" t="n">
+      <c r="Q5" t="n">
         <v>9374.669557944622</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
         <v>276.8699166878031</v>
       </c>
-      <c r="O5" t="n">
+      <c r="S5" t="n">
         <v>366.6020013147311</v>
       </c>
-      <c r="P5" t="n">
+      <c r="T5" t="n">
         <v>17.21490344390057</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="U5" t="n">
         <v>2.463546693298648</v>
       </c>
-      <c r="R5" t="n">
+      <c r="V5" t="n">
         <v>14.31054609935387</v>
       </c>
-      <c r="S5" t="n">
+      <c r="W5" t="n">
         <v>1.235904591147647</v>
       </c>
-      <c r="T5" t="n">
+      <c r="X5" t="n">
         <v>204.3424594184416</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>81
+(92,72)</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>8.7
+(19.8,3.8)</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -815,25 +941,31 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>46050.90522239159</v>
-      </c>
-      <c r="M6" t="n">
-        <v>9191.79744957916</v>
-      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
+        <v>46050.90522239159</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>9191.79744957916</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="n">
         <v>11.61284885745432</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="n">
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="n">
         <v>1.064938773683436</v>
       </c>
-      <c r="T6" t="n">
+      <c r="X6" t="n">
         <v>315.4171590574766</v>
       </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -859,25 +991,31 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
-        <v>65773.92710294698</v>
-      </c>
-      <c r="M7" t="n">
-        <v>10985.20703180743</v>
-      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
+        <v>65773.92710294698</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>10985.20703180743</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="n">
         <v>7.008953230507884</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="n">
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="n">
         <v>0.8456531620237618</v>
       </c>
-      <c r="T7" t="n">
+      <c r="X7" t="n">
         <v>450.5063500201848</v>
       </c>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -910,37 +1048,61 @@
         <v>65.07948742504992</v>
       </c>
       <c r="J8" t="n">
+        <v>83.39910513087202</v>
+      </c>
+      <c r="K8" t="n">
+        <v>50.78399434695405</v>
+      </c>
+      <c r="L8" t="n">
         <v>4.431981796208421</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
+        <v>10.70482092649276</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.834917442972895</v>
+      </c>
+      <c r="O8" t="n">
         <v>23.04998999891203</v>
       </c>
-      <c r="L8" t="n">
+      <c r="P8" t="n">
         <v>85268.60956677426</v>
       </c>
-      <c r="M8" t="n">
+      <c r="Q8" t="n">
         <v>14079.44017614436</v>
       </c>
-      <c r="N8" t="n">
+      <c r="R8" t="n">
         <v>1712.765360158157</v>
       </c>
-      <c r="O8" t="n">
+      <c r="S8" t="n">
         <v>909.5129508948302</v>
       </c>
-      <c r="P8" t="n">
+      <c r="T8" t="n">
         <v>11.14700398108137</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="U8" t="n">
         <v>2.88827239252185</v>
       </c>
-      <c r="R8" t="n">
+      <c r="V8" t="n">
         <v>25.91075052474916</v>
       </c>
-      <c r="S8" t="n">
+      <c r="W8" t="n">
         <v>1.047158156233841</v>
       </c>
-      <c r="T8" t="n">
+      <c r="X8" t="n">
         <v>460.9114030636447</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>65
+(83,51)</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>4.4
+(10.7,1.8)</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -967,25 +1129,31 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="n">
-        <v>99451.95742906225</v>
-      </c>
-      <c r="M9" t="n">
-        <v>13507.90593264003</v>
-      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
+        <v>99451.95742906225</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>13507.90593264003</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="n">
         <v>11.86373934705964</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="n">
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="n">
         <v>1.074221596434249</v>
       </c>
-      <c r="T9" t="n">
+      <c r="X9" t="n">
         <v>681.1777906100154</v>
       </c>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1011,25 +1179,31 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>127766.0304164031</v>
-      </c>
-      <c r="M10" t="n">
-        <v>15310.48896541679</v>
-      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
+        <v>127766.0304164031</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>15310.48896541679</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="n">
         <v>8.56661207435533</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="n">
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="n">
         <v>0.932809100998973</v>
       </c>
-      <c r="T10" t="n">
+      <c r="X10" t="n">
         <v>875.1097973726238</v>
       </c>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Some more code quality
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,20 +546,15 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>log_elastic_mod_mean</t>
+          <t>cross_section</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>cross_section</t>
+          <t>char_strength_disp</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>char_strength_disp</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>weibull_modulus_disp</t>
         </is>
@@ -635,18 +630,15 @@
         <v>20.07800784352419</v>
       </c>
       <c r="W2" t="n">
-        <v>1.944613387595852</v>
-      </c>
-      <c r="X2" t="n">
         <v>2.080328294037512</v>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>243
 (301,196)</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>3.5
 (6.3,1.9)</t>
@@ -723,18 +715,15 @@
         <v>6.397678740189672</v>
       </c>
       <c r="W3" t="n">
-        <v>1.653724468408931</v>
-      </c>
-      <c r="X3" t="n">
         <v>12.32874368763429</v>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>134
 (146,123)</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>7.8
 (13.0,4.7)</t>
@@ -811,18 +800,15 @@
         <v>8.352942400778611</v>
       </c>
       <c r="W4" t="n">
-        <v>1.605025141761029</v>
-      </c>
-      <c r="X4" t="n">
         <v>21.63104665880347</v>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="X4" t="inlineStr">
         <is>
           <t>148
 (176,124)</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>3.7
 (6.3,2.2)</t>
@@ -899,18 +885,15 @@
         <v>14.31054609935387</v>
       </c>
       <c r="W5" t="n">
-        <v>1.235904591147647</v>
-      </c>
-      <c r="X5" t="n">
         <v>204.3424594184416</v>
       </c>
-      <c r="Y5" t="inlineStr">
+      <c r="X5" t="inlineStr">
         <is>
           <t>81
 (92,72)</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>8.7
 (19.8,3.8)</t>
@@ -959,13 +942,10 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="n">
-        <v>1.064938773683436</v>
-      </c>
-      <c r="X6" t="n">
         <v>315.4171590574766</v>
       </c>
+      <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1009,13 +989,10 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
-        <v>0.8456531620237618</v>
-      </c>
-      <c r="X7" t="n">
         <v>450.5063500201848</v>
       </c>
+      <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1087,18 +1064,15 @@
         <v>25.91075052474916</v>
       </c>
       <c r="W8" t="n">
-        <v>1.047158156233841</v>
-      </c>
-      <c r="X8" t="n">
         <v>460.9114030636447</v>
       </c>
-      <c r="Y8" t="inlineStr">
+      <c r="X8" t="inlineStr">
         <is>
           <t>65
 (83,51)</t>
         </is>
       </c>
-      <c r="Z8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
         <is>
           <t>4.4
 (10.7,1.8)</t>
@@ -1147,13 +1121,10 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="n">
-        <v>1.074221596434249</v>
-      </c>
-      <c r="X9" t="n">
         <v>681.1777906100154</v>
       </c>
+      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1197,13 +1168,10 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
-        <v>0.932809100998973</v>
-      </c>
-      <c r="X10" t="n">
         <v>875.1097973726238</v>
       </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
small formatting changes for paper
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -635,13 +635,13 @@
       <c r="X2" t="inlineStr">
         <is>
           <t>243
-(301,196)</t>
+(196,301)</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
           <t>3.5
-(6.3,1.9)</t>
+(1.9,6.3)</t>
         </is>
       </c>
     </row>
@@ -720,13 +720,13 @@
       <c r="X3" t="inlineStr">
         <is>
           <t>134
-(146,123)</t>
+(123,146)</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
           <t>7.8
-(13.0,4.7)</t>
+(4.7,13.0)</t>
         </is>
       </c>
     </row>
@@ -805,13 +805,13 @@
       <c r="X4" t="inlineStr">
         <is>
           <t>148
-(176,124)</t>
+(124,176)</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
           <t>3.7
-(6.3,2.2)</t>
+(2.2,6.3)</t>
         </is>
       </c>
     </row>
@@ -890,13 +890,13 @@
       <c r="X5" t="inlineStr">
         <is>
           <t>81
-(92,72)</t>
+(72,92)</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
           <t>8.7
-(19.8,3.8)</t>
+(3.8,19.8)</t>
         </is>
       </c>
     </row>
@@ -1069,13 +1069,13 @@
       <c r="X8" t="inlineStr">
         <is>
           <t>65
-(83,51)</t>
+(51,83)</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
           <t>4.4
-(10.7,1.8)</t>
+(1.8,10.7)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New analysis for fibres
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,85 +476,90 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>valid_samples</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>char_strength</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>char_strength_95%_upper</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>char_strength_95%_lower</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>weibull_modulus</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>weibull_modulus_95%_upper</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>weibull_modulus_95%_lower</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Design Strength</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>mean_gage_V</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>mean_gage_SA</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>mean_effective_V</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>mean_effective_SA</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_mean</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_std</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_CV</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>cross_section</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>char_strength_disp</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>weibull_modulus_disp</t>
         </is>
@@ -588,60 +593,63 @@
         <v>90</v>
       </c>
       <c r="I2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" t="n">
         <v>243.0968542786452</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>301.1757812192096</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>196.2179041121504</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>3.462820561380488</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>6.33233774559996</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>1.893633397658162</v>
       </c>
-      <c r="O2" t="n">
-        <v>64.3939687516219</v>
-      </c>
       <c r="P2" t="n">
+        <v>103.10225151657</v>
+      </c>
+      <c r="Q2" t="n">
         <v>303.7279309294768</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>746.4895383827387</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>15.59242455167278</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>104.6741842613235</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>88.02649052883081</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>17.67396567275773</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>20.07800784352419</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>2.080328294037512</v>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>243
-(196,301)</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
+(196, 301)</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
         <is>
           <t>3.5
-(1.9,6.3)</t>
+(1.9, 6.3)</t>
         </is>
       </c>
     </row>
@@ -673,60 +681,63 @@
         <v>70</v>
       </c>
       <c r="I3" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" t="n">
         <v>134.1934515757539</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>145.8141782341235</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>123.4988439663269</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>7.827709892680903</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>12.99038824738473</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>4.716798374083251</v>
       </c>
-      <c r="O3" t="n">
-        <v>74.56024459595899</v>
-      </c>
       <c r="P3" t="n">
+        <v>91.82055347100366</v>
+      </c>
+      <c r="Q3" t="n">
         <v>2280.817582212344</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>2302.69316730171</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>28.77239337819473</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>142.7393917410353</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>45.05307813845685</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>2.882351201865095</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>6.397678740189672</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>12.32874368763429</v>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>134
-(123,146)</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
+(123, 146)</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
         <is>
           <t>7.8
-(4.7,13.0)</t>
+(4.7, 13.0)</t>
         </is>
       </c>
     </row>
@@ -758,60 +769,63 @@
         <v>70</v>
       </c>
       <c r="I4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" t="n">
         <v>147.6313386352384</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>176.0407780413132</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>123.8066111143724</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>3.732721538111613</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>6.257881243360847</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>2.226505991283302</v>
       </c>
-      <c r="O4" t="n">
-        <v>43.04876000792099</v>
-      </c>
       <c r="P4" t="n">
+        <v>66.61966475357605</v>
+      </c>
+      <c r="Q4" t="n">
         <v>4001.743631878642</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>3050.109475517258</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>137.5265212300033</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>300.4577935658554</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>40.27403487099166</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>3.364066935243426</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>8.352942400778611</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>21.63104665880347</v>
       </c>
-      <c r="X4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>148
-(124,176)</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
+(124, 176)</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
         <is>
           <t>3.7
-(2.2,6.3)</t>
+(2.2, 6.3)</t>
         </is>
       </c>
     </row>
@@ -843,60 +857,63 @@
         <v>40</v>
       </c>
       <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" t="n">
         <v>81.08861249799605</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>91.56091174079913</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>71.81408476429806</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>8.678824106185585</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>19.78614227873543</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>3.806805126791093</v>
       </c>
-      <c r="O5" t="n">
-        <v>47.72711205448898</v>
-      </c>
       <c r="P5" t="n">
+        <v>57.58762969041424</v>
+      </c>
+      <c r="Q5" t="n">
         <v>37803.35499241169</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>9374.669557944622</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>276.8699166878031</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>366.6020013147311</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>17.21490344390057</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>2.463546693298648</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>14.31054609935387</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>204.3424594184416</v>
       </c>
-      <c r="X5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>81
-(72,92)</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
+(72, 92)</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
         <is>
           <t>8.7
-(3.8,19.8)</t>
+(3.8, 19.8)</t>
         </is>
       </c>
     </row>
@@ -928,24 +945,25 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="n">
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="n">
         <v>46050.90522239159</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>9191.79744957916</v>
       </c>
-      <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
-      <c r="T6" t="n">
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="n">
         <v>11.61284885745432</v>
       </c>
-      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
-      <c r="W6" t="n">
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="n">
         <v>315.4171590574766</v>
       </c>
-      <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -975,24 +993,25 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="n">
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="n">
         <v>65773.92710294698</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>10985.20703180743</v>
       </c>
-      <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
-      <c r="T7" t="n">
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="n">
         <v>7.008953230507884</v>
       </c>
-      <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
-      <c r="W7" t="n">
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="n">
         <v>450.5063500201848</v>
       </c>
-      <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1022,60 +1041,63 @@
         <v>40</v>
       </c>
       <c r="I8" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" t="n">
         <v>65.07948742504992</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>83.39910513087202</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>50.78399434695405</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>4.431981796208421</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>10.70482092649276</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>1.834917442972895</v>
       </c>
-      <c r="O8" t="n">
-        <v>23.04998999891203</v>
-      </c>
       <c r="P8" t="n">
+        <v>33.29596589752567</v>
+      </c>
+      <c r="Q8" t="n">
         <v>85268.60956677426</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>14079.44017614436</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>1712.765360158157</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>909.5129508948302</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>11.14700398108137</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>2.88827239252185</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>25.91075052474916</v>
       </c>
-      <c r="W8" t="n">
+      <c r="X8" t="n">
         <v>460.9114030636447</v>
       </c>
-      <c r="X8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
         <is>
           <t>65
-(51,83)</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
+(51, 83)</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
         <is>
           <t>4.4
-(1.8,10.7)</t>
+(1.8, 10.7)</t>
         </is>
       </c>
     </row>
@@ -1107,24 +1129,25 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="n">
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="n">
         <v>99451.95742906225</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>13507.90593264003</v>
       </c>
-      <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
-      <c r="T9" t="n">
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="n">
         <v>11.86373934705964</v>
       </c>
-      <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
-      <c r="W9" t="n">
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="n">
         <v>681.1777906100154</v>
       </c>
-      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1154,24 +1177,25 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="n">
         <v>127766.0304164031</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>15310.48896541679</v>
       </c>
-      <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
         <v>8.56661207435533</v>
       </c>
-      <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
-      <c r="W10" t="n">
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="n">
         <v>875.1097973726238</v>
       </c>
-      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Handling different production methods
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,50 +516,55 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>mean_gage_V</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>mean_gage_SA</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>mean_effective_V</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>mean_effective_SA</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_mean</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_std</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>elastic_mod_CV</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>cross_section</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>char_strength_disp</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>weibull_modulus_disp</t>
         </is>
@@ -616,37 +621,42 @@
       <c r="P2" t="n">
         <v>103.10225151657</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>vitri</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
         <v>303.7279309294768</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>746.4895383827387</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>15.59242455167278</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>104.6741842613235</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>88.02649052883081</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>17.67396567275773</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>20.07800784352419</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Y2" t="n">
         <v>2.080328294037512</v>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>243
 (196, 301)</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>3.5
 (1.9, 6.3)</t>
@@ -704,37 +714,42 @@
       <c r="P3" t="n">
         <v>91.82055347100366</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>vitri</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
         <v>2280.817582212344</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>2302.69316730171</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>28.77239337819473</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>142.7393917410353</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>45.05307813845685</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>2.882351201865095</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>6.397678740189672</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Y3" t="n">
         <v>12.32874368763429</v>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>134
 (123, 146)</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>7.8
 (4.7, 13.0)</t>
@@ -792,37 +807,42 @@
       <c r="P4" t="n">
         <v>66.61966475357605</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>vitri</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
         <v>4001.743631878642</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>3050.109475517258</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>137.5265212300033</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>300.4577935658554</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>40.27403487099166</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>3.364066935243426</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>8.352942400778611</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>21.63104665880347</v>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>148
 (124, 176)</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="AA4" t="inlineStr">
         <is>
           <t>3.7
 (2.2, 6.3)</t>
@@ -880,37 +900,42 @@
       <c r="P5" t="n">
         <v>57.58762969041424</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>cast</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
         <v>37803.35499241169</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>9374.669557944622</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>276.8699166878031</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>366.6020013147311</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>17.21490344390057</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>2.463546693298648</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>14.31054609935387</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Y5" t="n">
         <v>204.3424594184416</v>
       </c>
-      <c r="Y5" t="inlineStr">
+      <c r="Z5" t="inlineStr">
         <is>
           <t>81
 (72, 92)</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr">
+      <c r="AA5" t="inlineStr">
         <is>
           <t>8.7
 (3.8, 19.8)</t>
@@ -946,24 +971,25 @@
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="n">
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
         <v>46050.90522239159</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>9191.79744957916</v>
       </c>
-      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="n">
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="n">
         <v>11.61284885745432</v>
       </c>
-      <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
-      <c r="X6" t="n">
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="n">
         <v>315.4171590574766</v>
       </c>
-      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -994,24 +1020,25 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="n">
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
         <v>65773.92710294698</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>10985.20703180743</v>
       </c>
-      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="n">
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="n">
         <v>7.008953230507884</v>
       </c>
-      <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
-      <c r="X7" t="n">
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="n">
         <v>450.5063500201848</v>
       </c>
-      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1064,37 +1091,42 @@
       <c r="P8" t="n">
         <v>33.29596589752567</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>cast</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
         <v>85268.60956677426</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>14079.44017614436</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>1712.765360158157</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>909.5129508948302</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>11.14700398108137</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>2.88827239252185</v>
       </c>
-      <c r="W8" t="n">
+      <c r="X8" t="n">
         <v>25.91075052474916</v>
       </c>
-      <c r="X8" t="n">
+      <c r="Y8" t="n">
         <v>460.9114030636447</v>
       </c>
-      <c r="Y8" t="inlineStr">
+      <c r="Z8" t="inlineStr">
         <is>
           <t>65
 (51, 83)</t>
         </is>
       </c>
-      <c r="Z8" t="inlineStr">
+      <c r="AA8" t="inlineStr">
         <is>
           <t>4.4
 (1.8, 10.7)</t>
@@ -1130,24 +1162,25 @@
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="n">
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
         <v>99451.95742906225</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>13507.90593264003</v>
       </c>
-      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="n">
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="n">
         <v>11.86373934705964</v>
       </c>
-      <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
-      <c r="X9" t="n">
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="n">
         <v>681.1777906100154</v>
       </c>
-      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1178,24 +1211,25 @@
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="n">
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="n">
         <v>127766.0304164031</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>15310.48896541679</v>
       </c>
-      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="n">
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="n">
         <v>8.56661207435533</v>
       </c>
-      <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
-      <c r="X10" t="n">
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="n">
         <v>875.1097973726238</v>
       </c>
-      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
stage 1 analysis depending on method
</commit_message>
<xml_diff>
--- a/Rod_test_analysis.xlsx
+++ b/Rod_test_analysis.xlsx
@@ -601,25 +601,25 @@
         <v>8</v>
       </c>
       <c r="J2" t="n">
-        <v>243.0968542786452</v>
+        <v>241.1142161815241</v>
       </c>
       <c r="K2" t="n">
-        <v>301.1757812192096</v>
+        <v>283.1250585464616</v>
       </c>
       <c r="L2" t="n">
-        <v>196.2179041121504</v>
+        <v>205.3370533265266</v>
       </c>
       <c r="M2" t="n">
-        <v>3.462820561380488</v>
+        <v>4.518851520511773</v>
       </c>
       <c r="N2" t="n">
-        <v>6.33233774559996</v>
+        <v>8.149026565380112</v>
       </c>
       <c r="O2" t="n">
-        <v>1.893633397658162</v>
+        <v>2.505823106674223</v>
       </c>
       <c r="P2" t="n">
-        <v>103.10225151657</v>
+        <v>124.958401618425</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -633,10 +633,10 @@
         <v>746.4895383827387</v>
       </c>
       <c r="T2" t="n">
-        <v>15.59242455167278</v>
+        <v>11.35491950195709</v>
       </c>
       <c r="U2" t="n">
-        <v>104.6741842613235</v>
+        <v>90.96286852303754</v>
       </c>
       <c r="V2" t="n">
         <v>88.02649052883081</v>
@@ -652,14 +652,14 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>243
-(196, 301)</t>
+          <t>241
+(205, 283)</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>3.5
-(1.9, 6.3)</t>
+          <t>4.5
+(2.5, 8.1)</t>
         </is>
       </c>
     </row>
@@ -694,25 +694,25 @@
         <v>10</v>
       </c>
       <c r="J3" t="n">
-        <v>134.1934515757539</v>
+        <v>134.1449701011463</v>
       </c>
       <c r="K3" t="n">
-        <v>145.8141782341235</v>
+        <v>144.5290465001201</v>
       </c>
       <c r="L3" t="n">
-        <v>123.4988439663269</v>
+        <v>124.5069654799285</v>
       </c>
       <c r="M3" t="n">
-        <v>7.827709892680903</v>
+        <v>8.768954184498069</v>
       </c>
       <c r="N3" t="n">
-        <v>12.99038824738473</v>
+        <v>14.44228397562113</v>
       </c>
       <c r="O3" t="n">
-        <v>4.716798374083251</v>
+        <v>5.324265719994549</v>
       </c>
       <c r="P3" t="n">
-        <v>91.82055347100366</v>
+        <v>95.60297344464202</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -726,10 +726,10 @@
         <v>2302.69316730171</v>
       </c>
       <c r="T3" t="n">
-        <v>28.77239337819473</v>
+        <v>24.51663412987911</v>
       </c>
       <c r="U3" t="n">
-        <v>142.7393917410353</v>
+        <v>133.2753708746945</v>
       </c>
       <c r="V3" t="n">
         <v>45.05307813845685</v>
@@ -746,13 +746,13 @@
       <c r="Z3" t="inlineStr">
         <is>
           <t>134
-(123, 146)</t>
+(125, 145)</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>7.8
-(4.7, 13.0)</t>
+          <t>8.8
+(5.3, 14.4)</t>
         </is>
       </c>
     </row>
@@ -787,25 +787,25 @@
         <v>10</v>
       </c>
       <c r="J4" t="n">
-        <v>147.6313386352384</v>
+        <v>146.8346489901402</v>
       </c>
       <c r="K4" t="n">
-        <v>176.0407780413132</v>
+        <v>170.1596387263386</v>
       </c>
       <c r="L4" t="n">
-        <v>123.8066111143724</v>
+        <v>126.7069811938922</v>
       </c>
       <c r="M4" t="n">
-        <v>3.732721538111613</v>
+        <v>4.42582981773189</v>
       </c>
       <c r="N4" t="n">
-        <v>6.257881243360847</v>
+        <v>7.335649771765482</v>
       </c>
       <c r="O4" t="n">
-        <v>2.226505991283302</v>
+        <v>2.670243289274487</v>
       </c>
       <c r="P4" t="n">
-        <v>66.61966475357605</v>
+        <v>75.05359092245527</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -819,10 +819,10 @@
         <v>3050.109475517258</v>
       </c>
       <c r="T4" t="n">
-        <v>137.5265212300033</v>
+        <v>110.0847982349058</v>
       </c>
       <c r="U4" t="n">
-        <v>300.4577935658554</v>
+        <v>269.5831474759362</v>
       </c>
       <c r="V4" t="n">
         <v>40.27403487099166</v>
@@ -838,14 +838,14 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>148
-(124, 176)</t>
+          <t>147
+(127, 170)</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>3.7
-(2.2, 6.3)</t>
+          <t>4.4
+(2.7, 7.3)</t>
         </is>
       </c>
     </row>
@@ -880,25 +880,25 @@
         <v>4</v>
       </c>
       <c r="J5" t="n">
-        <v>81.08861249799605</v>
+        <v>80.66718380179394</v>
       </c>
       <c r="K5" t="n">
-        <v>91.56091174079913</v>
+        <v>88.31352716578164</v>
       </c>
       <c r="L5" t="n">
-        <v>71.81408476429806</v>
+        <v>73.68287454193896</v>
       </c>
       <c r="M5" t="n">
-        <v>8.678824106185585</v>
+        <v>11.42761107958443</v>
       </c>
       <c r="N5" t="n">
-        <v>19.78614227873543</v>
+        <v>24.74932316464394</v>
       </c>
       <c r="O5" t="n">
-        <v>3.806805126791093</v>
+        <v>5.276519851371034</v>
       </c>
       <c r="P5" t="n">
-        <v>57.58762969041424</v>
+        <v>62.20391396429272</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -912,10 +912,10 @@
         <v>9374.669557944622</v>
       </c>
       <c r="T5" t="n">
-        <v>276.8699166878031</v>
+        <v>181.5729904224387</v>
       </c>
       <c r="U5" t="n">
-        <v>366.6020013147311</v>
+        <v>302.3052074333061</v>
       </c>
       <c r="V5" t="n">
         <v>17.21490344390057</v>
@@ -932,13 +932,13 @@
       <c r="Z5" t="inlineStr">
         <is>
           <t>81
-(72, 92)</t>
+(74, 88)</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>8.7
-(3.8, 19.8)</t>
+          <t>11.4
+(5.3, 24.7)</t>
         </is>
       </c>
     </row>
@@ -1071,25 +1071,25 @@
         <v>4</v>
       </c>
       <c r="J8" t="n">
-        <v>65.07948742504992</v>
+        <v>64.03564641645039</v>
       </c>
       <c r="K8" t="n">
-        <v>83.39910513087202</v>
+        <v>74.43443826719667</v>
       </c>
       <c r="L8" t="n">
-        <v>50.78399434695405</v>
+        <v>55.08960781369634</v>
       </c>
       <c r="M8" t="n">
-        <v>4.431981796208421</v>
+        <v>6.826103861777176</v>
       </c>
       <c r="N8" t="n">
-        <v>10.70482092649276</v>
+        <v>15.52715750065982</v>
       </c>
       <c r="O8" t="n">
-        <v>1.834917442972895</v>
+        <v>3.000915906841881</v>
       </c>
       <c r="P8" t="n">
-        <v>33.29596589752567</v>
+        <v>41.44291078397361</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -1103,10 +1103,10 @@
         <v>14079.44017614436</v>
       </c>
       <c r="T8" t="n">
-        <v>1712.765360158157</v>
+        <v>899.9401649186126</v>
       </c>
       <c r="U8" t="n">
-        <v>909.5129508948302</v>
+        <v>655.765974403018</v>
       </c>
       <c r="V8" t="n">
         <v>11.14700398108137</v>
@@ -1122,14 +1122,14 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>65
-(51, 83)</t>
+          <t>64
+(55, 74)</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>4.4
-(1.8, 10.7)</t>
+          <t>6.8
+(3.0, 15.5)</t>
         </is>
       </c>
     </row>

</xml_diff>